<commit_message>
+ Preparing for the release of Draco-6_2_0. + Update version number in CMakeLists.txt + Provide comments in ChangeLog. + Provide a release note and associated images and statistics. + Update draco.bib with citations for new/updated build tools and   vendors.
</commit_message>
<xml_diff>
--- a/doc/releases/historical-loc.xlsx
+++ b/doc/releases/historical-loc.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Draco-3_0_0</t>
   </si>
@@ -52,13 +52,55 @@
   </si>
   <si>
     <t>Draco-1_0_0</t>
+  </si>
+  <si>
+    <t>Using cloc</t>
+  </si>
+  <si>
+    <t>Draco-6_2_0</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Lisp</t>
+  </si>
+  <si>
+    <t>m4</t>
+  </si>
+  <si>
+    <t>CMake</t>
+  </si>
+  <si>
+    <t>Bourne Shell</t>
+  </si>
+  <si>
+    <t>Python</t>
+  </si>
+  <si>
+    <t>make</t>
+  </si>
+  <si>
+    <t>Perl</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>HTML</t>
+  </si>
+  <si>
+    <t>C/C++ Header</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,16 +108,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -83,14 +145,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -108,10 +186,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14349085591354221"/>
-          <c:y val="3.8956209421190775E-2"/>
-          <c:w val="0.82336896293760387"/>
-          <c:h val="0.81369719574526866"/>
+          <c:x val="0.14349085591354219"/>
+          <c:y val="3.8956209421190782E-2"/>
+          <c:w val="0.82336896293760375"/>
+          <c:h val="0.68738140627158451"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -135,9 +213,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -155,16 +233,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$8</c:f>
+              <c:f>Sheet1!$B$3:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>30665</c:v>
                 </c:pt>
@@ -182,6 +263,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>39210</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -206,9 +290,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -226,16 +310,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$8</c:f>
+              <c:f>Sheet1!$C$3:$C$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>12548</c:v>
                 </c:pt>
@@ -253,6 +340,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>22161</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>22481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -277,9 +367,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -297,16 +387,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$8</c:f>
+              <c:f>Sheet1!$D$3:$D$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>1237</c:v>
                 </c:pt>
@@ -324,6 +417,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>1443</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1494</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -348,9 +444,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$8</c:f>
-              <c:strCache>
-                <c:ptCount val="6"/>
+              <c:f>Sheet1!$A$3:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -368,16 +464,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$8</c:f>
+              <c:f>Sheet1!$E$3:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>24031</c:v>
                 </c:pt>
@@ -395,17 +494,20 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>43076</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>42763</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="55896704"/>
-        <c:axId val="56501760"/>
+        <c:axId val="80588160"/>
+        <c:axId val="80603008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55896704"/>
+        <c:axId val="80588160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -434,14 +536,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="56501760"/>
+        <c:crossAx val="80603008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="56501760"/>
+        <c:axId val="80603008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -467,7 +569,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55896704"/>
+        <c:crossAx val="80588160"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -478,9 +580,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.15741269056343798"/>
-          <c:y val="7.1347976239812136E-2"/>
-          <c:w val="0.2027590754054294"/>
+          <c:x val="0.14982261803351452"/>
+          <c:y val="5.023194498877686E-2"/>
+          <c:w val="0.26095010913054945"/>
           <c:h val="0.16607597734493715"/>
         </c:manualLayout>
       </c:layout>
@@ -499,8 +601,962 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$K$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C++</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$K$4:$K$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>29191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40639</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>42746</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>46202</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29280</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>69804</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72047</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Text</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$L$4:$L$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>10201</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13372</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31117</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35475</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>44318</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$M$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C/C++ Header</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$M$4:$M$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>26345</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22029</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22650</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23934</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11712</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22283</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21544</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$N$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lisp</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$N$4:$N$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="4">
+                  <c:v>6133</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6543</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6655</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$O$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>m4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$O$4:$O$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1185</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2302</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14066</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13833</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12273</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5901</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5876</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$P$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CMake</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$P$4:$P$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="5">
+                  <c:v>3265</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5241</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$Q$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bourne Shell</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Q$4:$Q$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>82645</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4372</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>135124</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>162263</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>152968</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4169</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4039</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$R$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Python</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$R$4:$R$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>612</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>828</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1532</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3382</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3184</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$S$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>make</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$S$4:$S$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>1265</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1539</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1417</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1464</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1482</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1855</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$T$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Perl</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$T$4:$T$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>224</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1828</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1828</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$U$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$U$4:$U$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>750</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$V$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>HTML</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$J$4:$J$10</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$V$4:$V$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7587</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:marker val="1"/>
+        <c:axId val="71772032"/>
+        <c:axId val="71780608"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="71772032"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Version</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Number</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71780608"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="71780608"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="80000"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Lines-of-Code</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="71772032"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.80020583190394512"/>
+          <c:y val="3.810323709536307E-2"/>
+          <c:w val="0.17577321386660247"/>
+          <c:h val="0.63588266851258979"/>
+        </c:manualLayout>
+      </c:layout>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup orientation="landscape"/>
+    <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -510,15 +1566,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>495299</xdr:colOff>
+      <xdr:colOff>933449</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -532,6 +1588,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -825,39 +1911,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A1:V11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row r="1" spans="1:22">
+      <c r="J1" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" ht="15.75" thickBot="1">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:22" ht="15.75" thickBot="1">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -873,8 +1965,47 @@
       <c r="E3">
         <v>24031</v>
       </c>
+      <c r="J3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -890,8 +2021,41 @@
       <c r="E4">
         <v>35213</v>
       </c>
+      <c r="J4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4">
+        <v>29191</v>
+      </c>
+      <c r="L4">
+        <v>10201</v>
+      </c>
+      <c r="M4">
+        <v>26345</v>
+      </c>
+      <c r="O4">
+        <v>1185</v>
+      </c>
+      <c r="Q4">
+        <v>82645</v>
+      </c>
+      <c r="R4">
+        <v>110</v>
+      </c>
+      <c r="S4">
+        <v>1265</v>
+      </c>
+      <c r="T4">
+        <v>224</v>
+      </c>
+      <c r="U4">
+        <v>82</v>
+      </c>
+      <c r="V4">
+        <v>50</v>
+      </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -907,8 +2071,41 @@
       <c r="E5">
         <v>37120</v>
       </c>
+      <c r="J5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K5">
+        <v>40639</v>
+      </c>
+      <c r="L5">
+        <v>13011</v>
+      </c>
+      <c r="M5">
+        <v>22029</v>
+      </c>
+      <c r="O5">
+        <v>2302</v>
+      </c>
+      <c r="Q5">
+        <v>4372</v>
+      </c>
+      <c r="R5">
+        <v>612</v>
+      </c>
+      <c r="S5">
+        <v>1539</v>
+      </c>
+      <c r="T5">
+        <v>180</v>
+      </c>
+      <c r="U5">
+        <v>88</v>
+      </c>
+      <c r="V5">
+        <v>7587</v>
+      </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -924,8 +2121,38 @@
       <c r="E6">
         <v>39817</v>
       </c>
+      <c r="J6" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>42746</v>
+      </c>
+      <c r="L6">
+        <v>13372</v>
+      </c>
+      <c r="M6">
+        <v>22650</v>
+      </c>
+      <c r="O6">
+        <v>14066</v>
+      </c>
+      <c r="Q6">
+        <v>135124</v>
+      </c>
+      <c r="R6">
+        <v>730</v>
+      </c>
+      <c r="S6">
+        <v>1417</v>
+      </c>
+      <c r="U6">
+        <v>105</v>
+      </c>
+      <c r="V6">
+        <v>55</v>
+      </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -941,8 +2168,35 @@
       <c r="E7">
         <v>21466</v>
       </c>
+      <c r="J7" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>46202</v>
+      </c>
+      <c r="L7">
+        <v>13901</v>
+      </c>
+      <c r="M7">
+        <v>23934</v>
+      </c>
+      <c r="O7">
+        <v>13833</v>
+      </c>
+      <c r="Q7">
+        <v>162263</v>
+      </c>
+      <c r="R7">
+        <v>828</v>
+      </c>
+      <c r="S7">
+        <v>1464</v>
+      </c>
+      <c r="V7">
+        <v>48</v>
+      </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -958,9 +2212,142 @@
       <c r="E8">
         <v>43076</v>
       </c>
+      <c r="J8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>29280</v>
+      </c>
+      <c r="L8">
+        <v>31117</v>
+      </c>
+      <c r="M8">
+        <v>11712</v>
+      </c>
+      <c r="N8">
+        <v>6133</v>
+      </c>
+      <c r="O8">
+        <v>12273</v>
+      </c>
+      <c r="Q8">
+        <v>152968</v>
+      </c>
+      <c r="R8">
+        <v>1532</v>
+      </c>
+      <c r="S8">
+        <v>1482</v>
+      </c>
+      <c r="U8">
+        <v>81</v>
+      </c>
+      <c r="V8">
+        <v>49</v>
+      </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>40006</v>
+      </c>
+      <c r="C9">
+        <v>22481</v>
+      </c>
+      <c r="D9">
+        <v>1494</v>
+      </c>
+      <c r="E9">
+        <v>42763</v>
+      </c>
+      <c r="J9" t="s">
+        <v>3</v>
+      </c>
+      <c r="K9">
+        <v>69804</v>
+      </c>
+      <c r="L9">
+        <v>35475</v>
+      </c>
+      <c r="M9">
+        <v>22283</v>
+      </c>
+      <c r="N9">
+        <v>6543</v>
+      </c>
+      <c r="O9">
+        <v>5901</v>
+      </c>
+      <c r="P9">
+        <v>3265</v>
+      </c>
+      <c r="Q9">
+        <v>4169</v>
+      </c>
+      <c r="R9">
+        <v>3382</v>
+      </c>
+      <c r="S9">
+        <v>1855</v>
+      </c>
+      <c r="T9">
+        <v>1828</v>
+      </c>
+      <c r="U9">
+        <v>696</v>
+      </c>
+      <c r="V9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" t="s">
+        <v>13</v>
+      </c>
+      <c r="K10">
+        <v>72047</v>
+      </c>
+      <c r="L10">
+        <v>44318</v>
+      </c>
+      <c r="M10">
+        <v>21544</v>
+      </c>
+      <c r="N10">
+        <v>6655</v>
+      </c>
+      <c r="O10">
+        <v>5876</v>
+      </c>
+      <c r="P10">
+        <v>5241</v>
+      </c>
+      <c r="Q10">
+        <v>4039</v>
+      </c>
+      <c r="R10">
+        <v>3184</v>
+      </c>
+      <c r="S10">
+        <v>1855</v>
+      </c>
+      <c r="T10">
+        <v>1828</v>
+      </c>
+      <c r="U10">
+        <v>750</v>
+      </c>
+      <c r="V10">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
+      <c r="J11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
+ Prepare for the release of Draco-6_5_0.   - Update ChangeLog, code metrics file, version number, and     release_process document.
</commit_message>
<xml_diff>
--- a/doc/releases/historical-loc.xlsx
+++ b/doc/releases/historical-loc.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="16080" windowHeight="13365"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="23850" windowHeight="15585"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="LOC" sheetId="1" r:id="rId1"/>
+    <sheet name="Coverage" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Draco-3_0_0</t>
   </si>
@@ -45,9 +48,6 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Draco-7_0_0</t>
-  </si>
-  <si>
     <t>Draco-2_0_0</t>
   </si>
   <si>
@@ -94,13 +94,85 @@
   </si>
   <si>
     <t>C/C++ Header</t>
+  </si>
+  <si>
+    <t>Draco-6_3_0</t>
+  </si>
+  <si>
+    <t>Draco-6_4_0</t>
+  </si>
+  <si>
+    <t>Draco-6_5_0</t>
+  </si>
+  <si>
+    <t>Fortran90</t>
+  </si>
+  <si>
+    <t>CUDA</t>
+  </si>
+  <si>
+    <t>Draco Coverage Metric</t>
+  </si>
+  <si>
+    <t>bullseyecoverage</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>draco-6_0_0</t>
+  </si>
+  <si>
+    <t>draco-6_1_0</t>
+  </si>
+  <si>
+    <t>draco-6_2_0</t>
+  </si>
+  <si>
+    <t>draco-6_3_0</t>
+  </si>
+  <si>
+    <t>draco-6_4_0</t>
+  </si>
+  <si>
+    <t>draco-6_5_0</t>
+  </si>
+  <si>
+    <t>12/2010</t>
+  </si>
+  <si>
+    <t>3/2011</t>
+  </si>
+  <si>
+    <t>8/2011</t>
+  </si>
+  <si>
+    <t>1/2012</t>
+  </si>
+  <si>
+    <t>6/2012</t>
+  </si>
+  <si>
+    <t>11/2012</t>
+  </si>
+  <si>
+    <t>Function Coverage</t>
+  </si>
+  <si>
+    <t>C/D Coverage</t>
+  </si>
+  <si>
+    <t>Draco Lines of Code</t>
+  </si>
+  <si>
+    <t>Using draco/tools/count_loc.sh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,8 +195,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -136,8 +215,14 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -154,17 +239,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -173,13 +276,29 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -189,17 +308,18 @@
           <c:x val="0.14349085591354219"/>
           <c:y val="3.8956209421190782E-2"/>
           <c:w val="0.82336896293760375"/>
-          <c:h val="0.68738140627158451"/>
+          <c:h val="0.86074440164367405"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$2</c:f>
+              <c:f>LOC!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -213,9 +333,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$A$5:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -236,16 +356,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$3:$B$9</c:f>
+              <c:f>LOC!$B$5:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>30665</c:v>
                 </c:pt>
@@ -266,17 +395,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>40006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40418</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40530</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>36936</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$2</c:f>
+              <c:f>LOC!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -290,9 +429,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$A$5:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -313,16 +452,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$C$9</c:f>
+              <c:f>LOC!$C$5:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>12548</c:v>
                 </c:pt>
@@ -343,17 +491,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>22481</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>22788</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22882</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>19098</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$2</c:f>
+              <c:f>LOC!$D$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -367,9 +525,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$A$5:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -390,16 +548,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$D$3:$D$9</c:f>
+              <c:f>LOC!$D$5:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1237</c:v>
                 </c:pt>
@@ -420,17 +587,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1494</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1549</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1547</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1585</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$E$2</c:f>
+              <c:f>LOC!$E$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -444,9 +621,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$A$9</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$A$5:$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -467,16 +644,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$E$3:$E$9</c:f>
+              <c:f>LOC!$E$5:$E$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>24031</c:v>
                 </c:pt>
@@ -497,20 +683,40 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>42763</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42466</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>42496</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>41997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="80588160"/>
-        <c:axId val="80603008"/>
+        <c:smooth val="0"/>
+        <c:axId val="49406976"/>
+        <c:axId val="82846272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80588160"/>
+        <c:axId val="49406976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -534,19 +740,24 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80603008"/>
+        <c:crossAx val="82846272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80603008"/>
+        <c:axId val="82846272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -566,10 +777,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80588160"/>
+        <c:crossAx val="49406976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -586,6 +800,7 @@
           <c:h val="0.16607597734493715"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:solidFill>
           <a:schemeClr val="bg1"/>
@@ -598,6 +813,8 @@
       </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -609,19 +826,40 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.4570387576261119E-2"/>
+          <c:y val="3.2534856219895589E-2"/>
+          <c:w val="0.7682846677351538"/>
+          <c:h val="0.83191439531597011"/>
+        </c:manualLayout>
+      </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$K$3</c:f>
+              <c:f>LOC!$K$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -632,9 +870,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -655,16 +893,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$K$4:$K$10</c:f>
+              <c:f>LOC!$K$5:$K$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>29191</c:v>
                 </c:pt>
@@ -685,17 +932,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>72047</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>72788</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>72905</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>67436</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$3</c:f>
+              <c:f>LOC!$L$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -706,9 +963,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -729,16 +986,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$L$4:$L$10</c:f>
+              <c:f>LOC!$L$5:$L$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10201</c:v>
                 </c:pt>
@@ -759,17 +1025,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>44318</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>55359</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>47634</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55728</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$M$3</c:f>
+              <c:f>LOC!$M$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -780,9 +1056,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -803,16 +1079,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$M$4:$M$10</c:f>
+              <c:f>LOC!$M$5:$M$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>26345</c:v>
                 </c:pt>
@@ -833,17 +1118,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>21544</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>20828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>20914</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21102</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$3</c:f>
+              <c:f>LOC!$N$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -854,9 +1149,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -877,16 +1172,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$N$4:$N$10</c:f>
+              <c:f>LOC!$N$5:$N$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="4">
                   <c:v>6133</c:v>
                 </c:pt>
@@ -895,17 +1199,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>6655</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6656</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11916</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11916</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$O$3</c:f>
+              <c:f>LOC!$O$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -916,9 +1230,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -939,16 +1253,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$4:$O$10</c:f>
+              <c:f>LOC!$O$5:$O$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1185</c:v>
                 </c:pt>
@@ -973,13 +1296,14 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$P$3</c:f>
+              <c:f>LOC!$P$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -990,9 +1314,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -1013,32 +1337,51 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$P$4:$P$10</c:f>
+              <c:f>LOC!$P$5:$P$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="5">
                   <c:v>3265</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>5241</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5153</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4797</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6788</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="6"/>
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Q$3</c:f>
+              <c:f>LOC!$Q$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1049,9 +1392,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -1072,16 +1415,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Q$4:$Q$10</c:f>
+              <c:f>LOC!$Q$5:$Q$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>82645</c:v>
                 </c:pt>
@@ -1102,17 +1454,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4039</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1399</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>548</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>514</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$3</c:f>
+              <c:f>LOC!$R$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1123,9 +1485,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -1146,16 +1508,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$R$4:$R$10</c:f>
+              <c:f>LOC!$R$5:$R$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>110</c:v>
                 </c:pt>
@@ -1176,17 +1547,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3184</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3154</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2197</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2197</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="8"/>
           <c:order val="8"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$S$3</c:f>
+              <c:f>LOC!$S$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1197,9 +1578,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -1220,16 +1601,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$S$4:$S$10</c:f>
+              <c:f>LOC!$S$5:$S$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>1265</c:v>
                 </c:pt>
@@ -1250,17 +1640,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1855</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>344</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="9"/>
           <c:order val="9"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$T$3</c:f>
+              <c:f>LOC!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1271,9 +1671,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -1294,16 +1694,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$4:$T$10</c:f>
+              <c:f>LOC!$T$5:$T$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>224</c:v>
                 </c:pt>
@@ -1315,17 +1724,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1828</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1828</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8330</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8330</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="10"/>
           <c:order val="10"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$U$3</c:f>
+              <c:f>LOC!$U$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1336,9 +1755,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -1359,16 +1778,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$U$4:$U$10</c:f>
+              <c:f>LOC!$U$5:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>82</c:v>
                 </c:pt>
@@ -1386,17 +1814,27 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>750</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>633</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>652</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>800</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="11"/>
           <c:order val="11"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$V$3</c:f>
+              <c:f>LOC!$V$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1407,9 +1845,9 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$J$4:$J$10</c:f>
-              <c:strCache>
-                <c:ptCount val="7"/>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>Draco-1_0_0</c:v>
                 </c:pt>
@@ -1430,16 +1868,25 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$V$4:$V$10</c:f>
+              <c:f>LOC!$V$5:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>50</c:v>
                 </c:pt>
@@ -1459,21 +1906,176 @@
                   <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LOC!$W$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fortran90</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LOC!$W$5:$W$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="8">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>118</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>LOC!$X$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>CUDA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>LOC!$J$5:$J$14</c:f>
+              <c:strCache>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>Draco-1_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Draco-2_0_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Draco-3_0_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Draco-4_0_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Draco-5_0_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Draco-6_5_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>LOC!$X$5:$X$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="9">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="71772032"/>
-        <c:axId val="71780608"/>
+        <c:smooth val="0"/>
+        <c:axId val="53347840"/>
+        <c:axId val="82848576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71772032"/>
+        <c:axId val="53347840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:title>
           <c:tx>
@@ -1497,20 +2099,25 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71780608"/>
+        <c:crossAx val="82848576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71780608"/>
+        <c:axId val="82848576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="80000"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:title>
@@ -1530,10 +2137,13 @@
             </c:rich>
           </c:tx>
           <c:layout/>
+          <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="71772032"/>
+        <c:crossAx val="53347840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1544,14 +2154,259 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.80020583190394512"/>
-          <c:y val="3.810323709536307E-2"/>
-          <c:w val="0.17577321386660247"/>
-          <c:h val="0.63588266851258979"/>
+          <c:x val="0.87171475963203637"/>
+          <c:y val="2.63817022872141E-2"/>
+          <c:w val="0.117295391139191"/>
+          <c:h val="0.55128375713722333"/>
         </c:manualLayout>
       </c:layout>
+      <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.7393864579712923E-2"/>
+          <c:y val="3.5372419888249823E-2"/>
+          <c:w val="0.89861735319614733"/>
+          <c:h val="0.88481348086517209"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Coverage!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Function Coverage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]Coverage!$B$6:$G$6</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>draco-6_1_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>draco-6_5_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Coverage!$B$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Coverage!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>C/D Coverage</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>[1]Coverage!$B$6:$G$6</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>draco-6_0_0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>draco-6_1_0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>draco-6_2_0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>draco-6_3_0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>draco-6_4_0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>draco-6_5_0</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Coverage!$B$9:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="58667008"/>
+        <c:axId val="56080000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="58667008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="56080000"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="56080000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="58667008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.7269462321776037E-2"/>
+          <c:y val="0.77691608551775837"/>
+          <c:w val="0.21475489079846755"/>
+          <c:h val="0.11522364710566144"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
@@ -1566,15 +2421,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>933449</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:colOff>843801</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>151837</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>414617</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>33616</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1595,16 +2450,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>19049</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>19049</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>590549</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>156883</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>161924</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>11205</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>83483</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1624,6 +2479,127 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>761999</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="LOC"/>
+      <sheetName val="Coverage"/>
+      <sheetName val="Sheet3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>draco-6_0_0</v>
+          </cell>
+          <cell r="C6" t="str">
+            <v>draco-6_1_0</v>
+          </cell>
+          <cell r="D6" t="str">
+            <v>draco-6_2_0</v>
+          </cell>
+          <cell r="E6" t="str">
+            <v>draco-6_3_0</v>
+          </cell>
+          <cell r="F6" t="str">
+            <v>draco-6_4_0</v>
+          </cell>
+          <cell r="G6" t="str">
+            <v>draco-6_5_0</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>Function Coverage</v>
+          </cell>
+          <cell r="B8">
+            <v>0.91</v>
+          </cell>
+          <cell r="C8">
+            <v>0.96</v>
+          </cell>
+          <cell r="D8">
+            <v>0.95</v>
+          </cell>
+          <cell r="E8">
+            <v>0.95</v>
+          </cell>
+          <cell r="F8">
+            <v>0.97</v>
+          </cell>
+          <cell r="G8">
+            <v>0.96</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>C/D Coverage</v>
+          </cell>
+          <cell r="B9">
+            <v>0.79</v>
+          </cell>
+          <cell r="C9">
+            <v>0.8</v>
+          </cell>
+          <cell r="D9">
+            <v>0.79</v>
+          </cell>
+          <cell r="E9">
+            <v>0.8</v>
+          </cell>
+          <cell r="F9">
+            <v>0.81</v>
+          </cell>
+          <cell r="G9">
+            <v>0.8</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1701,6 +2677,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1735,6 +2712,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1910,14 +2888,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
@@ -1927,411 +2905,414 @@
     <col min="10" max="10" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="J1" s="1" t="s">
-        <v>12</v>
-      </c>
+    <row r="1" spans="1:24" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5"/>
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5"/>
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
     </row>
-    <row r="2" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="J3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="J4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="X4" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5">
         <v>30665</v>
       </c>
-      <c r="C3">
+      <c r="C5">
         <v>12548</v>
       </c>
-      <c r="D3">
+      <c r="D5">
         <v>1237</v>
       </c>
-      <c r="E3">
+      <c r="E5">
         <v>24031</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>35273</v>
-      </c>
-      <c r="C4">
-        <v>18698</v>
-      </c>
-      <c r="D4">
-        <v>1481</v>
-      </c>
-      <c r="E4">
-        <v>35213</v>
-      </c>
-      <c r="J4" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4">
-        <v>29191</v>
-      </c>
-      <c r="L4">
-        <v>10201</v>
-      </c>
-      <c r="M4">
-        <v>26345</v>
-      </c>
-      <c r="O4">
-        <v>1185</v>
-      </c>
-      <c r="Q4">
-        <v>82645</v>
-      </c>
-      <c r="R4">
-        <v>110</v>
-      </c>
-      <c r="S4">
-        <v>1265</v>
-      </c>
-      <c r="T4">
-        <v>224</v>
-      </c>
-      <c r="U4">
-        <v>82</v>
-      </c>
-      <c r="V4">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>37374</v>
-      </c>
-      <c r="C5">
-        <v>20153</v>
-      </c>
-      <c r="D5">
-        <v>1667</v>
-      </c>
-      <c r="E5">
-        <v>37120</v>
       </c>
       <c r="J5" t="s">
         <v>10</v>
       </c>
       <c r="K5">
+        <v>29191</v>
+      </c>
+      <c r="L5">
+        <v>10201</v>
+      </c>
+      <c r="M5">
+        <v>26345</v>
+      </c>
+      <c r="O5">
+        <v>1185</v>
+      </c>
+      <c r="Q5">
+        <v>82645</v>
+      </c>
+      <c r="R5">
+        <v>110</v>
+      </c>
+      <c r="S5">
+        <v>1265</v>
+      </c>
+      <c r="T5">
+        <v>224</v>
+      </c>
+      <c r="U5">
+        <v>82</v>
+      </c>
+      <c r="V5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>35273</v>
+      </c>
+      <c r="C6">
+        <v>18698</v>
+      </c>
+      <c r="D6">
+        <v>1481</v>
+      </c>
+      <c r="E6">
+        <v>35213</v>
+      </c>
+      <c r="J6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6">
         <v>40639</v>
       </c>
-      <c r="L5">
+      <c r="L6">
         <v>13011</v>
       </c>
-      <c r="M5">
+      <c r="M6">
         <v>22029</v>
       </c>
-      <c r="O5">
+      <c r="O6">
         <v>2302</v>
       </c>
-      <c r="Q5">
+      <c r="Q6">
         <v>4372</v>
       </c>
-      <c r="R5">
+      <c r="R6">
         <v>612</v>
       </c>
-      <c r="S5">
+      <c r="S6">
         <v>1539</v>
       </c>
-      <c r="T5">
+      <c r="T6">
         <v>180</v>
       </c>
-      <c r="U5">
+      <c r="U6">
         <v>88</v>
       </c>
-      <c r="V5">
+      <c r="V6">
         <v>7587</v>
       </c>
     </row>
-    <row r="6" spans="1:22">
-      <c r="A6" t="s">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>37374</v>
+      </c>
+      <c r="C7">
+        <v>20153</v>
+      </c>
+      <c r="D7">
+        <v>1667</v>
+      </c>
+      <c r="E7">
+        <v>37120</v>
+      </c>
+      <c r="J7" t="s">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>42746</v>
+      </c>
+      <c r="L7">
+        <v>13372</v>
+      </c>
+      <c r="M7">
+        <v>22650</v>
+      </c>
+      <c r="O7">
+        <v>14066</v>
+      </c>
+      <c r="Q7">
+        <v>135124</v>
+      </c>
+      <c r="R7">
+        <v>730</v>
+      </c>
+      <c r="S7">
+        <v>1417</v>
+      </c>
+      <c r="U7">
+        <v>105</v>
+      </c>
+      <c r="V7">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>1</v>
       </c>
-      <c r="B6">
+      <c r="B8">
         <v>40035</v>
       </c>
-      <c r="C6">
+      <c r="C8">
         <v>21884</v>
       </c>
-      <c r="D6">
+      <c r="D8">
         <v>1902</v>
       </c>
-      <c r="E6">
+      <c r="E8">
         <v>39817</v>
       </c>
-      <c r="J6" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>42746</v>
-      </c>
-      <c r="L6">
-        <v>13372</v>
-      </c>
-      <c r="M6">
-        <v>22650</v>
-      </c>
-      <c r="O6">
-        <v>14066</v>
-      </c>
-      <c r="Q6">
-        <v>135124</v>
-      </c>
-      <c r="R6">
-        <v>730</v>
-      </c>
-      <c r="S6">
-        <v>1417</v>
-      </c>
-      <c r="U6">
-        <v>105</v>
-      </c>
-      <c r="V6">
-        <v>55</v>
+      <c r="J8" t="s">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>46202</v>
+      </c>
+      <c r="L8">
+        <v>13901</v>
+      </c>
+      <c r="M8">
+        <v>23934</v>
+      </c>
+      <c r="O8">
+        <v>13833</v>
+      </c>
+      <c r="Q8">
+        <v>162263</v>
+      </c>
+      <c r="R8">
+        <v>828</v>
+      </c>
+      <c r="S8">
+        <v>1464</v>
+      </c>
+      <c r="V8">
+        <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
-      <c r="A7" t="s">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
-      <c r="B7">
+      <c r="B9">
         <v>21106</v>
       </c>
-      <c r="C7">
+      <c r="C9">
         <v>12479</v>
       </c>
-      <c r="D7">
+      <c r="D9">
         <v>628</v>
       </c>
-      <c r="E7">
+      <c r="E9">
         <v>21466</v>
       </c>
-      <c r="J7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7">
-        <v>46202</v>
-      </c>
-      <c r="L7">
-        <v>13901</v>
-      </c>
-      <c r="M7">
-        <v>23934</v>
-      </c>
-      <c r="O7">
-        <v>13833</v>
-      </c>
-      <c r="Q7">
-        <v>162263</v>
-      </c>
-      <c r="R7">
-        <v>828</v>
-      </c>
-      <c r="S7">
-        <v>1464</v>
-      </c>
-      <c r="V7">
-        <v>48</v>
+      <c r="J9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>29280</v>
+      </c>
+      <c r="L9">
+        <v>31117</v>
+      </c>
+      <c r="M9">
+        <v>11712</v>
+      </c>
+      <c r="N9">
+        <v>6133</v>
+      </c>
+      <c r="O9">
+        <v>12273</v>
+      </c>
+      <c r="Q9">
+        <v>152968</v>
+      </c>
+      <c r="R9">
+        <v>1532</v>
+      </c>
+      <c r="S9">
+        <v>1482</v>
+      </c>
+      <c r="U9">
+        <v>81</v>
+      </c>
+      <c r="V9">
+        <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
-      <c r="A8" t="s">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B8">
+      <c r="B10">
         <v>39210</v>
       </c>
-      <c r="C8">
+      <c r="C10">
         <v>22161</v>
       </c>
-      <c r="D8">
+      <c r="D10">
         <v>1443</v>
       </c>
-      <c r="E8">
+      <c r="E10">
         <v>43076</v>
       </c>
-      <c r="J8" t="s">
-        <v>2</v>
-      </c>
-      <c r="K8">
-        <v>29280</v>
-      </c>
-      <c r="L8">
-        <v>31117</v>
-      </c>
-      <c r="M8">
-        <v>11712</v>
-      </c>
-      <c r="N8">
-        <v>6133</v>
-      </c>
-      <c r="O8">
-        <v>12273</v>
-      </c>
-      <c r="Q8">
-        <v>152968</v>
-      </c>
-      <c r="R8">
-        <v>1532</v>
-      </c>
-      <c r="S8">
-        <v>1482</v>
-      </c>
-      <c r="U8">
-        <v>81</v>
-      </c>
-      <c r="V8">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>40006</v>
-      </c>
-      <c r="C9">
-        <v>22481</v>
-      </c>
-      <c r="D9">
-        <v>1494</v>
-      </c>
-      <c r="E9">
-        <v>42763</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>3</v>
       </c>
-      <c r="K9">
+      <c r="K10">
         <v>69804</v>
       </c>
-      <c r="L9">
+      <c r="L10">
         <v>35475</v>
       </c>
-      <c r="M9">
+      <c r="M10">
         <v>22283</v>
       </c>
-      <c r="N9">
+      <c r="N10">
         <v>6543</v>
       </c>
-      <c r="O9">
+      <c r="O10">
         <v>5901</v>
       </c>
-      <c r="P9">
+      <c r="P10">
         <v>3265</v>
       </c>
-      <c r="Q9">
+      <c r="Q10">
         <v>4169</v>
       </c>
-      <c r="R9">
+      <c r="R10">
         <v>3382</v>
-      </c>
-      <c r="S9">
-        <v>1855</v>
-      </c>
-      <c r="T9">
-        <v>1828</v>
-      </c>
-      <c r="U9">
-        <v>696</v>
-      </c>
-      <c r="V9">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10">
-        <v>72047</v>
-      </c>
-      <c r="L10">
-        <v>44318</v>
-      </c>
-      <c r="M10">
-        <v>21544</v>
-      </c>
-      <c r="N10">
-        <v>6655</v>
-      </c>
-      <c r="O10">
-        <v>5876</v>
-      </c>
-      <c r="P10">
-        <v>5241</v>
-      </c>
-      <c r="Q10">
-        <v>4039</v>
-      </c>
-      <c r="R10">
-        <v>3184</v>
       </c>
       <c r="S10">
         <v>1855</v>
@@ -2340,15 +3321,234 @@
         <v>1828</v>
       </c>
       <c r="U10">
-        <v>750</v>
+        <v>696</v>
       </c>
       <c r="V10">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>40006</v>
+      </c>
+      <c r="C11">
+        <v>22481</v>
+      </c>
+      <c r="D11">
+        <v>1494</v>
+      </c>
+      <c r="E11">
+        <v>42763</v>
+      </c>
       <c r="J11" t="s">
-        <v>9</v>
+        <v>12</v>
+      </c>
+      <c r="K11">
+        <v>72047</v>
+      </c>
+      <c r="L11">
+        <v>44318</v>
+      </c>
+      <c r="M11">
+        <v>21544</v>
+      </c>
+      <c r="N11">
+        <v>6655</v>
+      </c>
+      <c r="O11">
+        <v>5876</v>
+      </c>
+      <c r="P11">
+        <v>5241</v>
+      </c>
+      <c r="Q11">
+        <v>4039</v>
+      </c>
+      <c r="R11">
+        <v>3184</v>
+      </c>
+      <c r="S11">
+        <v>1855</v>
+      </c>
+      <c r="T11">
+        <v>1828</v>
+      </c>
+      <c r="U11">
+        <v>750</v>
+      </c>
+      <c r="V11">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12">
+        <v>40418</v>
+      </c>
+      <c r="C12">
+        <v>22788</v>
+      </c>
+      <c r="D12">
+        <v>1549</v>
+      </c>
+      <c r="E12">
+        <v>42466</v>
+      </c>
+      <c r="J12" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12">
+        <v>72788</v>
+      </c>
+      <c r="L12">
+        <v>55359</v>
+      </c>
+      <c r="M12">
+        <v>20828</v>
+      </c>
+      <c r="N12">
+        <v>6656</v>
+      </c>
+      <c r="P12">
+        <v>5153</v>
+      </c>
+      <c r="Q12">
+        <v>1399</v>
+      </c>
+      <c r="R12">
+        <v>3154</v>
+      </c>
+      <c r="S12">
+        <v>532</v>
+      </c>
+      <c r="T12">
+        <v>1828</v>
+      </c>
+      <c r="U12">
+        <v>633</v>
+      </c>
+      <c r="V12">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13">
+        <v>40530</v>
+      </c>
+      <c r="C13">
+        <v>22882</v>
+      </c>
+      <c r="D13">
+        <v>1547</v>
+      </c>
+      <c r="E13">
+        <v>42496</v>
+      </c>
+      <c r="J13" t="s">
+        <v>26</v>
+      </c>
+      <c r="K13">
+        <v>72905</v>
+      </c>
+      <c r="L13">
+        <v>47634</v>
+      </c>
+      <c r="M13">
+        <v>20914</v>
+      </c>
+      <c r="N13">
+        <v>11916</v>
+      </c>
+      <c r="P13">
+        <v>4797</v>
+      </c>
+      <c r="Q13">
+        <v>548</v>
+      </c>
+      <c r="R13">
+        <v>2197</v>
+      </c>
+      <c r="S13">
+        <v>344</v>
+      </c>
+      <c r="T13">
+        <v>8330</v>
+      </c>
+      <c r="U13">
+        <v>652</v>
+      </c>
+      <c r="V13">
+        <v>45</v>
+      </c>
+      <c r="W13">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14">
+        <v>36936</v>
+      </c>
+      <c r="C14">
+        <v>19098</v>
+      </c>
+      <c r="D14">
+        <v>1585</v>
+      </c>
+      <c r="E14">
+        <v>41997</v>
+      </c>
+      <c r="J14" t="s">
+        <v>27</v>
+      </c>
+      <c r="K14">
+        <v>67436</v>
+      </c>
+      <c r="L14">
+        <v>55728</v>
+      </c>
+      <c r="M14">
+        <v>21102</v>
+      </c>
+      <c r="N14">
+        <v>11916</v>
+      </c>
+      <c r="P14">
+        <v>6788</v>
+      </c>
+      <c r="Q14">
+        <v>514</v>
+      </c>
+      <c r="R14">
+        <v>2197</v>
+      </c>
+      <c r="S14">
+        <v>205</v>
+      </c>
+      <c r="T14">
+        <v>8330</v>
+      </c>
+      <c r="U14">
+        <v>800</v>
+      </c>
+      <c r="V14">
+        <v>45</v>
+      </c>
+      <c r="W14">
+        <v>118</v>
+      </c>
+      <c r="X14">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2359,24 +3559,143 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="7" width="13.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
+      <c r="B7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0.91</v>
+      </c>
+      <c r="C8" s="8">
+        <v>0.96</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="E8" s="8">
+        <v>0.95</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0.97</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="C9" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="D9" s="8">
+        <v>0.79</v>
+      </c>
+      <c r="E9" s="8">
+        <v>0.8</v>
+      </c>
+      <c r="F9" s="8">
+        <v>0.81</v>
+      </c>
+      <c r="G9" s="8">
+        <v>0.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>